<commit_message>
added order column to model
</commit_message>
<xml_diff>
--- a/dist/erngenturis.xlsx
+++ b/dist/erngenturis.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="91">
   <si>
     <t>ernstats</t>
   </si>
@@ -25,7 +25,7 @@
     <t>ERN Genturis Stats</t>
   </si>
   <si>
-    <t>Descriptives on enrolled patients and data providers (v1.1.0, 2022-06-17)</t>
+    <t>Descriptives on enrolled patients and data providers (v1.1.1, 2022-10-10)</t>
   </si>
   <si>
     <t>dataproviders</t>
@@ -97,6 +97,9 @@
     <t>value</t>
   </si>
   <si>
+    <t>valueOrder</t>
+  </si>
+  <si>
     <t>component</t>
   </si>
   <si>
@@ -145,6 +148,9 @@
     <t>raw data value</t>
   </si>
   <si>
+    <t>integer specifying the order of a value in an array (ideal for tables, charts)</t>
+  </si>
+  <si>
     <t>name of the component that the current will be used in</t>
   </si>
   <si>
@@ -163,6 +169,9 @@
     <t>hyperlink</t>
   </si>
   <si>
+    <t>int</t>
+  </si>
+  <si>
     <t>text</t>
   </si>
   <si>
@@ -226,34 +235,34 @@
     <t>visible</t>
   </si>
   <si>
-    <t>auto</t>
+    <t>defaultValue</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25160</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25464</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C41206</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C172872</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70896</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C68642</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25160</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C172872</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70896</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25464</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C68642</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C41206</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C68643</t>
@@ -654,7 +663,7 @@
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -683,7 +692,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
@@ -692,7 +701,7 @@
         <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -730,7 +739,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -738,40 +747,40 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -782,10 +791,10 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -803,7 +812,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="K2" t="b">
         <v>1</v>
@@ -817,10 +826,10 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -829,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K3" t="b">
         <v>1</v>
@@ -843,10 +852,10 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -855,7 +864,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="K4" t="b">
         <v>1</v>
@@ -869,10 +878,10 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -881,7 +890,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K5" t="b">
         <v>1</v>
@@ -895,10 +904,10 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -907,7 +916,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K6" t="b">
         <v>1</v>
@@ -921,10 +930,10 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -933,7 +942,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="K7" t="b">
         <v>1</v>
@@ -947,10 +956,10 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -959,7 +968,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K8" t="b">
         <v>1</v>
@@ -973,7 +982,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -982,7 +991,7 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="K9" t="b">
         <v>1</v>
@@ -996,7 +1005,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -1005,7 +1014,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K10" t="b">
         <v>1</v>
@@ -1019,10 +1028,10 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -1031,7 +1040,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K11" t="b">
         <v>1</v>
@@ -1045,10 +1054,10 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -1079,9 +1088,6 @@
       <c r="K13" t="b">
         <v>1</v>
       </c>
-      <c r="L13" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
@@ -1091,10 +1097,10 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -1114,10 +1120,10 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -1143,10 +1149,10 @@
         <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -1158,7 +1164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1166,10 +1172,10 @@
         <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -1180,8 +1186,11 @@
       <c r="K17" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1189,10 +1198,10 @@
         <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -1201,6 +1210,29 @@
         <v>1</v>
       </c>
       <c r="K18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1219,122 +1251,122 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1345,96 +1377,96 @@
         <v>53</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E7" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added table for storing inclusion criteria
</commit_message>
<xml_diff>
--- a/dist/erngenturis.xlsx
+++ b/dist/erngenturis.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="119">
   <si>
     <t>ernstats</t>
   </si>
@@ -25,30 +25,42 @@
     <t>ERN Genturis Stats</t>
   </si>
   <si>
-    <t>Descriptives on enrolled patients and data providers (v1.2.0, 2022-12-01)</t>
+    <t>Descriptives on enrolled patients and data providers (v1.3.0, 2023-02-20)</t>
   </si>
   <si>
     <t>dataproviders</t>
   </si>
   <si>
+    <t>inclusionCriteria</t>
+  </si>
+  <si>
     <t>stats</t>
   </si>
   <si>
     <t>Data Providers</t>
   </si>
   <si>
+    <t>Inclusion criteria</t>
+  </si>
+  <si>
     <t>Summary Statistics</t>
   </si>
   <si>
     <t>All affiliated data providers (intitutions, hospitals, etc.)</t>
   </si>
   <si>
+    <t>Define or modify inclusion criteria for each subgroup</t>
+  </si>
+  <si>
     <t>Stats used in the dashboard</t>
   </si>
   <si>
     <t>ernstats_dataproviders</t>
   </si>
   <si>
+    <t>ernstats_inclusionCriteria</t>
+  </si>
+  <si>
     <t>ernstats_stats</t>
   </si>
   <si>
@@ -109,15 +121,30 @@
     <t>longitude</t>
   </si>
   <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>groupID</t>
+  </si>
+  <si>
+    <t>groupName</t>
+  </si>
+  <si>
+    <t>criteria</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
     <t>title</t>
   </si>
   <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>valueOrder</t>
   </si>
   <si>
@@ -163,6 +190,24 @@
     <t>An imaginary great circle on the surface of a heavenly body passing through the poles at right angles to the equator.</t>
   </si>
   <si>
+    <t>table row identifier</t>
+  </si>
+  <si>
+    <t>A unique ID used to identify a group</t>
+  </si>
+  <si>
+    <t>Name of the group</t>
+  </si>
+  <si>
+    <t>A variable to identify criteria for a specific group (e.g., "genes", "disease", etc.)</t>
+  </si>
+  <si>
+    <t>values used to select rows (IDs, codes, etc.)</t>
+  </si>
+  <si>
+    <t>additional context that describes the criteria</t>
+  </si>
+  <si>
     <t>title to be rendered into the app (e.g., section heading, component title, table heading, etc)</t>
   </si>
   <si>
@@ -274,34 +319,34 @@
     <t>defaultValue</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25341</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25160</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C68642</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C68643</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C70896</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C51875</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25464</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C51875</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C68642</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70896</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C68643</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25341</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25160</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C172872</t>
@@ -696,13 +741,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -723,7 +768,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -731,16 +776,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -751,10 +796,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -765,10 +810,24 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -778,7 +837,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -786,57 +845,57 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -856,13 +915,13 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -876,13 +935,13 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -894,21 +953,21 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -920,15 +979,15 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -940,15 +999,15 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -960,21 +1019,21 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="K7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -986,24 +1045,24 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="K8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -1015,50 +1074,50 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="K9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
         <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" t="b">
-        <v>1</v>
-      </c>
-      <c r="K10" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -1070,15 +1129,15 @@
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -1090,21 +1149,21 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -1116,21 +1175,21 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="K13" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -1142,18 +1201,18 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="K14" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -1165,21 +1224,21 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="K15" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -1191,21 +1250,21 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -1217,24 +1276,24 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="K17" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -1246,24 +1305,24 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="K18" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -1275,47 +1334,50 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="K19" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>84</v>
+      </c>
+      <c r="K20" t="s">
         <v>29</v>
-      </c>
-      <c r="C20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" t="b">
-        <v>1</v>
-      </c>
-      <c r="J20" t="s">
-        <v>69</v>
-      </c>
-      <c r="K20" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
       </c>
       <c r="E21" t="b">
         <v>1</v>
@@ -1324,21 +1386,18 @@
         <v>0</v>
       </c>
       <c r="I21" t="b">
-        <v>1</v>
-      </c>
-      <c r="L21" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -1348,49 +1407,34 @@
       </c>
       <c r="I22" t="b">
         <v>1</v>
-      </c>
-      <c r="J22" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
       </c>
-      <c r="F23" t="b">
-        <v>1</v>
-      </c>
-      <c r="G23" t="b">
-        <v>1</v>
-      </c>
       <c r="H23" t="b">
         <v>1</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
-      </c>
-      <c r="J23" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -1402,18 +1446,18 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
@@ -1424,22 +1468,19 @@
       <c r="I25" t="b">
         <v>1</v>
       </c>
-      <c r="J25" t="s">
-        <v>70</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
+      <c r="K25" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -1450,19 +1491,19 @@
       <c r="I26" t="b">
         <v>1</v>
       </c>
-      <c r="J26" t="s">
-        <v>65</v>
+      <c r="K26" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -1473,8 +1514,175 @@
       <c r="I27" t="b">
         <v>1</v>
       </c>
-      <c r="J27" t="s">
-        <v>71</v>
+      <c r="K27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+      <c r="L28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" t="b">
+        <v>0</v>
+      </c>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E32" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>85</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1492,242 +1700,242 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="E2" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="E3" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="E4" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="D5" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="E5" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="D7" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="E7" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="D8" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="D9" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="E9" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="D10" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="D11" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="E11" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="D12" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="E12" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>